<commit_message>
+ edit data, add more get iteration history
</commit_message>
<xml_diff>
--- a/uts/data-facial-wash.xlsx
+++ b/uts/data-facial-wash.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\py_code\Fuzzy-Logic\uts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC21D97-42E4-48D8-B78E-C6FACA6EDE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE73E80-76EC-4142-9228-A1745E580C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,9 +107,6 @@
     <t>Simple Moisturising Facial Wash</t>
   </si>
   <si>
-    <t>SK-II Facial Treatment Cleansing Gel</t>
-  </si>
-  <si>
     <t>Pigeon Facial Foam</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>Wardah Nature Daily Mineral Plus Clarifying Facial Foam</t>
+  </si>
+  <si>
+    <t>Innisfree Bija Trouble Facial Foam</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,13 +847,13 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B20" s="4">
-        <v>320000</v>
+        <v>60000</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D20" s="6">
         <v>3.9929999999999999</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="4">
         <v>9450</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="4">
         <v>31635</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="4">
         <v>38000</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="4">
         <v>16900</v>
@@ -932,7 +932,7 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="4">
         <v>31927</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="4">
         <v>32400</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="4">
         <v>100000</v>
@@ -983,7 +983,7 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="4">
         <v>32000</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="4">
         <v>18250</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="4">
         <v>32500</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="4">
         <v>65000</v>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="4">
         <v>28000</v>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="4">
         <v>84915</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="4">
         <v>32580</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="4">
         <v>32000</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" s="4">
         <v>15875</v>

</xml_diff>